<commit_message>
edit robots.txt search excel file
</commit_message>
<xml_diff>
--- a/documents/robots.txt 조사.xlsx
+++ b/documents/robots.txt 조사.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User1\Documents\GitHub\Readers\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Capstone\Readers\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C29169-2C1B-4781-8CBD-9055524A4849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70825015-16CF-4232-84FA-DA5C8587E5E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{ED2EB456-9463-4B33-B09E-261F692F9DF1}"/>
+    <workbookView xWindow="-10605" yWindow="3495" windowWidth="21600" windowHeight="11385" xr2:uid="{ED2EB456-9463-4B33-B09E-261F692F9DF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="87">
   <si>
     <t>네이버</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -291,6 +291,31 @@
   </si>
   <si>
     <t>웹툰페이지는 허용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모두 비허용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disallow: /</t>
+  </si>
+  <si>
+    <t>모두 허용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User-agent: * </t>
+  </si>
+  <si>
+    <t>Allow : /</t>
+  </si>
+  <si>
+    <t>존재x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>존재 및 모두 허용</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -658,12 +683,12 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,28 +735,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>79</v>
       </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
       <c r="E2" t="s">
         <v>36</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
       </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
       <c r="H2" t="s">
         <v>78</v>
       </c>
+      <c r="J2" t="s">
+        <v>85</v>
+      </c>
       <c r="K2" t="s">
         <v>37</v>
       </c>
       <c r="L2" t="s">
         <v>36</v>
       </c>
+      <c r="M2" t="s">
+        <v>86</v>
+      </c>
       <c r="N2" t="s">
         <v>75</v>
       </c>
@@ -739,7 +779,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
@@ -749,6 +792,9 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
+      <c r="G3" t="s">
+        <v>83</v>
+      </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
@@ -762,10 +808,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
+      <c r="G4" t="s">
+        <v>84</v>
+      </c>
       <c r="I4" t="s">
         <v>38</v>
       </c>
@@ -773,7 +825,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>20</v>
       </c>
@@ -796,7 +848,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>21</v>
       </c>
@@ -819,7 +871,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>22</v>
       </c>
@@ -830,7 +882,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>23</v>
       </c>
@@ -841,7 +893,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>24</v>
       </c>
@@ -849,7 +901,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>25</v>
       </c>
@@ -857,12 +909,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>16</v>
       </c>
@@ -870,7 +922,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>26</v>
       </c>
@@ -878,7 +930,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>27</v>
       </c>
@@ -886,7 +938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>28</v>
       </c>
@@ -894,7 +946,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>29</v>
       </c>
@@ -902,7 +954,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>30</v>
       </c>
@@ -910,7 +962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>31</v>
       </c>
@@ -918,7 +970,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>32</v>
       </c>
@@ -926,7 +978,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>33</v>
       </c>
@@ -934,67 +986,67 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N27" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N29" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N30" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
       <c r="N31" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N33" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="14:14" x14ac:dyDescent="0.3">
       <c r="N34" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Update login and sign in activity
Update login and sign in activity
</commit_message>
<xml_diff>
--- a/documents/robots.txt 조사.xlsx
+++ b/documents/robots.txt 조사.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User1\Documents\GitHub\Readers\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C29169-2C1B-4781-8CBD-9055524A4849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED465FF-6D06-479D-B4C9-595F9D50D11D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{ED2EB456-9463-4B33-B09E-261F692F9DF1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>네이버</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -102,10 +102,6 @@
     <t>Disallow:</t>
   </si>
   <si>
-    <t>모두 비허용</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>lezhin.com/robots.txt</t>
   </si>
   <si>
@@ -291,6 +287,31 @@
   </si>
   <si>
     <t>웹툰페이지는 허용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disallow: /</t>
+  </si>
+  <si>
+    <t>모두비허용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User-agent: * </t>
+  </si>
+  <si>
+    <t>Allow : /</t>
+  </si>
+  <si>
+    <t>모두 허용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>존재x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>됨</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -658,7 +679,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -711,37 +732,58 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
       </c>
       <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" t="s">
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>78</v>
-      </c>
-      <c r="K2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
-        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -749,6 +791,9 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
@@ -756,110 +801,116 @@
         <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L5" t="s">
         <v>16</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="N11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -867,136 +918,136 @@
         <v>16</v>
       </c>
       <c r="N12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.45">
       <c r="N31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="14:14" x14ac:dyDescent="0.45">
       <c r="N33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="14:14" x14ac:dyDescent="0.45">
       <c r="N34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>